<commit_message>
Change `firstValueIsKey` to `numColumnKeys`
</commit_message>
<xml_diff>
--- a/Sample Project/Assets/Workspace/Test_excel.xlsx
+++ b/Sample Project/Assets/Workspace/Test_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hunter\Documents\Project Documents\Git\Lync\Sample Project\Assets\Workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C76664E-D659-43C5-99C1-EBA2E8753B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7D146D-531F-4DF9-8058-01C50AF357CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8895" yWindow="3720" windowWidth="32250" windowHeight="17445" xr2:uid="{72F043A4-F0E0-44B4-AD79-65D8A11EF329}"/>
+    <workbookView xWindow="14475" yWindow="3435" windowWidth="32250" windowHeight="17445" xr2:uid="{72F043A4-F0E0-44B4-AD79-65D8A11EF329}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Charlie</t>
+  </si>
+  <si>
+    <t>Baz</t>
   </si>
 </sst>
 </file>
@@ -89,9 +92,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,56 +408,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32E7A12F-E602-4E6A-AC3E-715A9951CBB7}">
-  <dimension ref="C4:E7"/>
+  <dimension ref="C4:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
-  </cols>
   <sheetData>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C4" s="1" t="s">
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>2</v>
       </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>512</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5">
         <v>64</v>
       </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>256</v>
       </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
     </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>128</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7">
         <v>16</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix sheet names with spaces
</commit_message>
<xml_diff>
--- a/Sample Project/Assets/Workspace/Test_excel.xlsx
+++ b/Sample Project/Assets/Workspace/Test_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hunter\Documents\Project Documents\Git\Lync\Sample Project\Assets\Workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7D146D-531F-4DF9-8058-01C50AF357CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1752F3-5170-4E7B-929E-6DA03CBFB385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14475" yWindow="3435" windowWidth="32250" windowHeight="17445" xr2:uid="{72F043A4-F0E0-44B4-AD79-65D8A11EF329}"/>
+    <workbookView xWindow="12210" yWindow="2055" windowWidth="32250" windowHeight="17445" xr2:uid="{72F043A4-F0E0-44B4-AD79-65D8A11EF329}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Potentially fix Meta deletions, or break more stuff
</commit_message>
<xml_diff>
--- a/Sample Project/Assets/Workspace/Test_excel.xlsx
+++ b/Sample Project/Assets/Workspace/Test_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hunter\Documents\Project Documents\Git\Lync\Sample Project\Assets\Workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1752F3-5170-4E7B-929E-6DA03CBFB385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006570DE-9228-4E06-89F4-DEDBE256FE84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12210" yWindow="2055" windowWidth="32250" windowHeight="17445" xr2:uid="{72F043A4-F0E0-44B4-AD79-65D8A11EF329}"/>
+    <workbookView xWindow="12555" yWindow="2400" windowWidth="32250" windowHeight="17445" xr2:uid="{72F043A4-F0E0-44B4-AD79-65D8A11EF329}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -411,7 +411,7 @@
   <dimension ref="C4:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>